<commit_message>
calendar unions for all instruments, reference_date replaced by trade_date removed get_start_date from base_instrument removed get_frame() adding calculate_spot_date implemented EOM flag for date arithmetics Changed tenor 1B to 1D introducing get_fwd_rate_aligned renamed curve.plot() to curve.plot_fwd() added yc_calendar added "ZeroRate" instrument ability to generate empty price ladder option to explicitly provide convention for yc_curve.plot() curve plotting now use no compounting do not allow dates before 1/3/1900 stub generation na --> null in spreadsheets
</commit_message>
<xml_diff>
--- a/conventions.xlsx
+++ b/conventions.xlsx
@@ -17,14 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t>3M</t>
   </si>
   <si>
-    <t>1B</t>
-  </si>
-  <si>
     <t>6M</t>
   </si>
   <si>
@@ -86,6 +83,15 @@
   </si>
   <si>
     <t>Notes:</t>
+  </si>
+  <si>
+    <t>EURLIBOR1M</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>1D</t>
   </si>
 </sst>
 </file>
@@ -471,7 +477,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,24 +492,24 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -515,55 +521,55 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
@@ -572,18 +578,18 @@
         <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>0</v>
@@ -592,15 +598,15 @@
         <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>0</v>
@@ -609,15 +615,15 @@
         <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>0</v>
@@ -626,15 +632,15 @@
         <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>0</v>
@@ -643,24 +649,41 @@
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>19</v>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:3">

</xml_diff>

<commit_message>
changed curve naming conventions
</commit_message>
<xml_diff>
--- a/conventions.xlsx
+++ b/conventions.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A785DED-77BD-4509-A832-D6F3DB344EE3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="13920" windowHeight="4950"/>
+    <workbookView xWindow="0" yWindow="132" windowWidth="13920" windowHeight="4956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conventions" sheetId="1" r:id="rId1"/>
@@ -25,15 +26,6 @@
     <t>6M</t>
   </si>
   <si>
-    <t>USDLIBOR3M</t>
-  </si>
-  <si>
-    <t>USDLIBOR6M</t>
-  </si>
-  <si>
-    <t>USD-USDOIS</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -52,27 +44,9 @@
     <t>ACT360</t>
   </si>
   <si>
-    <t>USDLIBOR12M</t>
-  </si>
-  <si>
-    <t>USDOIS</t>
-  </si>
-  <si>
-    <t>GBP-USDOIS</t>
-  </si>
-  <si>
     <t>12M</t>
   </si>
   <si>
-    <t>GBP-GBPSONIA</t>
-  </si>
-  <si>
-    <t>GBPSONIA</t>
-  </si>
-  <si>
-    <t>GBPLIBOR3M</t>
-  </si>
-  <si>
     <t>ACT365</t>
   </si>
   <si>
@@ -85,20 +59,47 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>EURLIBOR1M</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
     <t>1D</t>
+  </si>
+  <si>
+    <t>USD.LIBOR.3M</t>
+  </si>
+  <si>
+    <t>USD.LIBOR.6M</t>
+  </si>
+  <si>
+    <t>USD.LIBOR.12M</t>
+  </si>
+  <si>
+    <t>USD.OIS</t>
+  </si>
+  <si>
+    <t>USD/USD.OIS</t>
+  </si>
+  <si>
+    <t>GBP/USD.OIS</t>
+  </si>
+  <si>
+    <t>GBP.SONIA</t>
+  </si>
+  <si>
+    <t>GBP/GBP.SONIA</t>
+  </si>
+  <si>
+    <t>GBP.LIBOR.3M</t>
+  </si>
+  <si>
+    <t>EUR.LIBOR.1M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +186,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -231,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,9 +272,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -297,6 +324,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -472,61 +517,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -538,465 +583,465 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>

</xml_diff>